<commit_message>
update Review_Log_V_2.0.xlsx after Reviewing
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Review_Log_V_2.0.xlsx
+++ b/Documents/Second_Week/Review_Log_V_2.0.xlsx
@@ -433,12 +433,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,6 +455,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -495,15 +504,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -814,7 +814,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H16"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,713 +832,718 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>1.2</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="6">
         <v>2</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="15"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="20"/>
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="16"/>
-      <c r="K4" s="17"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="20"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="21">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="21">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="21">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="21">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="19" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="16"/>
-      <c r="K8" s="17"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="21">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
       <c r="I10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="A11" s="21">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="19" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="21">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="21">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="21">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="16"/>
-      <c r="K14" s="17"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="21">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20">
+      <c r="A16" s="23">
         <v>15</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="11">
         <v>2.5</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="9" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="22"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23">
+      <c r="A17" s="26">
         <v>15</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="28">
         <v>2</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23">
+      <c r="A18" s="26">
         <v>16</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25" t="s">
+      <c r="E18" s="28"/>
+      <c r="F18" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="26" t="s">
+      <c r="H18" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="31" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="29" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="6">
         <v>1</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="5"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="8">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="30"/>
-      <c r="K20" s="7"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="30"/>
-      <c r="K21" s="7"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="8">
         <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>1.2</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="30"/>
-      <c r="K22" s="7"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+      <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>1.2</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
       <c r="I23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="30"/>
-      <c r="K23" s="7"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="A24" s="8">
         <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>1.3</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
       <c r="I24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="30"/>
-      <c r="K24" s="7"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
       <c r="I25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="30"/>
-      <c r="K25" s="7"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="A26" s="8">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
       <c r="I26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="30"/>
-      <c r="K26" s="7"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+      <c r="A27" s="8">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
       <c r="I27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="30"/>
-      <c r="K27" s="7"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+      <c r="A28" s="8">
         <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
       <c r="I28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="30"/>
-      <c r="K28" s="7"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="9"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+      <c r="A29" s="8">
         <v>28</v>
       </c>
       <c r="B29" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
       <c r="I29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="30"/>
-      <c r="K29" s="7"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+      <c r="A30" s="8">
         <v>30</v>
       </c>
       <c r="B30" s="2">
         <v>4.3</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
       <c r="I30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="30"/>
-      <c r="K30" s="7"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="A31" s="8">
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
       <c r="I31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="30"/>
-      <c r="K31" s="7"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="9"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+      <c r="A32" s="8">
         <v>32</v>
       </c>
       <c r="B32" s="2">
         <v>5</v>
       </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
       <c r="I32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="30"/>
-      <c r="K32" s="7"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="9"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="A33" s="8">
         <v>33</v>
       </c>
       <c r="B33" s="2">
         <v>6.1</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
       <c r="I33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J33" s="30"/>
-      <c r="K33" s="7"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="9"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
+      <c r="A34" s="10">
         <v>34</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="11">
         <v>6.2</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="9" t="s">
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J34" s="31"/>
-      <c r="K34" s="10"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C19:C34"/>
+    <mergeCell ref="E2:E16"/>
+    <mergeCell ref="E19:E34"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="D19:D34"/>
     <mergeCell ref="F19:F34"/>
     <mergeCell ref="G19:G34"/>
     <mergeCell ref="H19:H34"/>
@@ -1547,11 +1552,6 @@
     <mergeCell ref="F2:F16"/>
     <mergeCell ref="G2:G16"/>
     <mergeCell ref="H2:H16"/>
-    <mergeCell ref="C19:C34"/>
-    <mergeCell ref="E2:E16"/>
-    <mergeCell ref="E19:E34"/>
-    <mergeCell ref="C2:C16"/>
-    <mergeCell ref="D19:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Review_Log_V_2.0.xlsxw_Log_V_2.0 after Reviewing
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Review_Log_V_2.0.xlsx
+++ b/Documents/Second_Week/Review_Log_V_2.0.xlsx
@@ -433,18 +433,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,9 +449,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -504,6 +495,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -814,7 +814,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19:J34"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,718 +832,713 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1.2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="29">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
       <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="17"/>
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="20"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="17"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="17"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="22" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="20"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
       <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="20"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="18">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="18">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="22" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="18">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="A13" s="18">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
       <c r="I13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="20"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="18">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
       <c r="I14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="18">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="20"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23">
+      <c r="A16" s="20">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="9">
         <v>2.5</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="11" t="s">
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="25"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="22"/>
     </row>
     <row r="17" spans="1:11" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26">
+      <c r="A17" s="23">
         <v>15</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="25">
         <v>2</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="29" t="s">
+      <c r="H17" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="31" t="s">
+      <c r="K17" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26">
+      <c r="A18" s="23">
         <v>16</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28" t="s">
+      <c r="E18" s="25"/>
+      <c r="F18" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="29" t="s">
+      <c r="H18" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="31" t="s">
+      <c r="K18" s="28" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="4"/>
+      <c r="C19" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="29">
         <v>1</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="7"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
       <c r="I20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="9"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
       <c r="I21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="9"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>1.2</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
       <c r="I22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="9"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>1.2</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
       <c r="I23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="9"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>1.3</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
       <c r="I24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="9"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
       <c r="I25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="9"/>
+      <c r="J25" s="30"/>
+      <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
       <c r="I26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="9"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
       <c r="I27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="9"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
       <c r="I28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="9"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
       <c r="B29" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
       <c r="I29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="3"/>
-      <c r="K29" s="9"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="6">
         <v>30</v>
       </c>
       <c r="B30" s="2">
         <v>4.3</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J30" s="3"/>
-      <c r="K30" s="9"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="6">
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
       <c r="I31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="9"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="6">
         <v>32</v>
       </c>
       <c r="B32" s="2">
         <v>5</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
       <c r="I32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="9"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="7"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="6">
         <v>33</v>
       </c>
       <c r="B33" s="2">
         <v>6.1</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="9"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="7"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="10">
+      <c r="A34" s="8">
         <v>34</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="9">
         <v>6.2</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="11" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="J34" s="12"/>
-      <c r="K34" s="13"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C19:C34"/>
-    <mergeCell ref="E2:E16"/>
-    <mergeCell ref="E19:E34"/>
-    <mergeCell ref="C2:C16"/>
-    <mergeCell ref="D19:D34"/>
     <mergeCell ref="F19:F34"/>
     <mergeCell ref="G19:G34"/>
     <mergeCell ref="H19:H34"/>
@@ -1552,6 +1547,11 @@
     <mergeCell ref="F2:F16"/>
     <mergeCell ref="G2:G16"/>
     <mergeCell ref="H2:H16"/>
+    <mergeCell ref="C19:C34"/>
+    <mergeCell ref="E2:E16"/>
+    <mergeCell ref="E19:E34"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="D19:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>